<commit_message>
cambios de la version 4
</commit_message>
<xml_diff>
--- a/resultados/precios_gpt3.xlsx
+++ b/resultados/precios_gpt3.xlsx
@@ -461,24 +461,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "At the evening offering I arose up from my humiliation, even with my garment and my robe torn; and I fell on my knees, and spread out my hands to Yahweh my God;" I find that word "garment" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "At the evening offering I arose up from my humiliation, even with my garment and my robe torn; and I fell on my knees, and spread out my hands to Yahweh my God;"
+Word: "garment"
+Class: </t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>315</v>
+        <v>217</v>
       </c>
       <c r="D2" t="n">
         <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>320</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3">
@@ -487,24 +491,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "It shall be to them as a false divination in their sight, who have sworn oaths to them; but he brings iniquity to memory, that they may be taken." I find that word "divination" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "It shall be to them as a false divination in their sight, who have sworn oaths to them; but he brings iniquity to memory, that they may be taken."
+Word: "divination"
+Class: </t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>313</v>
+        <v>215</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>318</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4">
@@ -513,24 +521,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "You have received gifts among men, yes, among the rebellious also, that Yah God might dwell there." I find that word "gifts" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "You have received gifts among men, yes, among the rebellious also, that Yah God might dwell there."
+Word: "gifts"
+Class: </t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>297</v>
+        <v>199</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>302</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5">
@@ -539,24 +551,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Therefore he poured the fierceness of his anger on him, and the strength of battle; and it set him on fire all around, but he didn't know; and it burned him, but he didn't take it to heart."" I find that word "strength" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Therefore he poured the fierceness of his anger on him, and the strength of battle; and it set him on fire all around, but he didn't know; and it burned him, but he didn't take it to heart.""
+Word: "strength"
+Class: </t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>324</v>
+        <v>226</v>
       </c>
       <c r="D5" t="n">
         <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>329</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6">
@@ -565,24 +581,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "The seventh angel sounded, and great voices in heaven followed, saying, "The kingdom of the world has become the Kingdom of our Lord, and of his Christ." I find that word "voices" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "The seventh angel sounded, and great voices in heaven followed, saying, "The kingdom of the world has become the Kingdom of our Lord, and of his Christ."
+Word: "voices"
+Class: </t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>309</v>
+        <v>211</v>
       </c>
       <c r="D6" t="n">
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>314</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7">
@@ -591,24 +611,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "who by the mouth of your servant, David, said, 'Why do the nations rage, and the peoples plot a vain thing?" I find that word "rage" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "who by the mouth of your servant, David, said, 'Why do the nations rage, and the peoples plot a vain thing?"
+Word: "rage"
+Class: </t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>302</v>
+        <v>204</v>
       </c>
       <c r="D7" t="n">
         <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>307</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8">
@@ -617,24 +641,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "'You shall keep my Sabbaths, and reverence my sanctuary; I am Yahweh." I find that word "Sabbaths" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "'You shall keep my Sabbaths, and reverence my sanctuary; I am Yahweh."
+Word: "Sabbaths"
+Class: </t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>295</v>
+        <v>197</v>
       </c>
       <c r="D8" t="n">
         <v>5</v>
       </c>
       <c r="E8" t="n">
-        <v>300</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9">
@@ -643,24 +671,28 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Neither have we inheritance in the son of Jesse!" I find that word "Jesse" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Neither have we inheritance in the son of Jesse!"
+Word: "Jesse"
+Class: </t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>286</v>
+        <v>188</v>
       </c>
       <c r="D9" t="n">
         <v>5</v>
       </c>
       <c r="E9" t="n">
-        <v>291</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10">
@@ -669,24 +701,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Only the firstborn among animals, which is made a firstborn to Yahweh, no man may dedicate it; whether an ox or sheep, it is Yahweh's." I find that word "animals" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Only the firstborn among animals, which is made a firstborn to Yahweh, no man may dedicate it; whether an ox or sheep, it is Yahweh's."
+Word: "animals"
+Class: </t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>313</v>
+        <v>215</v>
       </c>
       <c r="D10" t="n">
         <v>5</v>
       </c>
       <c r="E10" t="n">
-        <v>318</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11">
@@ -695,24 +731,28 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Don't be desirous of his dainties, since they are deceitful food." I find that word "dainties" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Don't be desirous of his dainties, since they are deceitful food."
+Word: "dainties"
+Class: </t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>296</v>
+        <v>198</v>
       </c>
       <c r="D11" t="n">
         <v>5</v>
       </c>
       <c r="E11" t="n">
-        <v>301</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12">
@@ -721,24 +761,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "The floods have lifted up, Yahweh, the floods have lifted up their voice." I find that word "voice" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "The floods have lifted up, Yahweh, the floods have lifted up their voice."
+Word: "voice"
+Class: </t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>293</v>
+        <v>195</v>
       </c>
       <c r="D12" t="n">
         <v>5</v>
       </c>
       <c r="E12" t="n">
-        <v>298</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13">
@@ -747,24 +791,28 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "He has walled up my way so that I can't pass, and has set darkness in my paths." I find that word "darkness" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "He has walled up my way so that I can't pass, and has set darkness in my paths."
+Word: "darkness"
+Class: </t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>298</v>
+        <v>200</v>
       </c>
       <c r="D13" t="n">
         <v>5</v>
       </c>
       <c r="E13" t="n">
-        <v>303</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14">
@@ -773,24 +821,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Now, behold, the hand of the Lord is on you, and you will be blind, not seeing the sun for a season!"" I find that word "behold" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Now, behold, the hand of the Lord is on you, and you will be blind, not seeing the sun for a season!""
+Word: "behold"
+Class: </t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>304</v>
+        <v>206</v>
       </c>
       <c r="D14" t="n">
         <v>5</v>
       </c>
       <c r="E14" t="n">
-        <v>309</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15">
@@ -799,24 +851,28 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "But the flesh of the bull, and its skin, and its dung, you shall burn with fire outside of the camp: it is a sin offering." I find that word "camp" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "But the flesh of the bull, and its skin, and its dung, you shall burn with fire outside of the camp: it is a sin offering."
+Word: "camp"
+Class: </t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>307</v>
+        <v>209</v>
       </c>
       <c r="D15" t="n">
         <v>5</v>
       </c>
       <c r="E15" t="n">
-        <v>312</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16">
@@ -825,24 +881,28 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "But if her husband altogether hold his peace at her from day to day, then he establishes all her vows, or all her bonds, which are on her: he has established them, because he held his peace at her in the day that he heard them." I find that word "bonds" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "But if her husband altogether hold his peace at her from day to day, then he establishes all her vows, or all her bonds, which are on her: he has established them, because he held his peace at her in the day that he heard them."
+Word: "bonds"
+Class: </t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>328</v>
+        <v>230</v>
       </c>
       <c r="D16" t="n">
         <v>5</v>
       </c>
       <c r="E16" t="n">
-        <v>333</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17">
@@ -851,24 +911,28 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Teach me your statutes." I find that word "statutes" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Teach me your statutes."
+Word: "statutes"
+Class: </t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>282</v>
+        <v>184</v>
       </c>
       <c r="D17" t="n">
         <v>5</v>
       </c>
       <c r="E17" t="n">
-        <v>287</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18">
@@ -877,24 +941,28 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "They talk about laying snares secretly." I find that word "snares" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "They talk about laying snares secretly."
+Word: "snares"
+Class: </t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>286</v>
+        <v>188</v>
       </c>
       <c r="D18" t="n">
         <v>5</v>
       </c>
       <c r="E18" t="n">
-        <v>291</v>
+        <v>193</v>
       </c>
     </row>
     <row r="19">
@@ -903,24 +971,28 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "But he who prophesies speaks to men for their edification, exhortation, and consolation." I find that word "exhortation" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "But he who prophesies speaks to men for their edification, exhortation, and consolation."
+Word: "exhortation"
+Class: </t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>298</v>
+        <v>200</v>
       </c>
       <c r="D19" t="n">
         <v>5</v>
       </c>
       <c r="E19" t="n">
-        <v>303</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20">
@@ -929,24 +1001,28 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Then Tattenai, the governor beyond the River, Shetharbozenai, and their companions, because Darius the king had sent a decree, did accordingly with all diligence." I find that word "River" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Then Tattenai, the governor beyond the River, Shetharbozenai, and their companions, because Darius the king had sent a decree, did accordingly with all diligence."
+Word: "River"
+Class: </t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>312</v>
+        <v>214</v>
       </c>
       <c r="D20" t="n">
         <v>5</v>
       </c>
       <c r="E20" t="n">
-        <v>317</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21">
@@ -955,24 +1031,28 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "They are a perverse and crooked generation." I find that word "generation" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "They are a perverse and crooked generation."
+Word: "generation"
+Class: </t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>283</v>
+        <v>185</v>
       </c>
       <c r="D21" t="n">
         <v>5</v>
       </c>
       <c r="E21" t="n">
-        <v>288</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22">
@@ -981,24 +1061,28 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Then let our faces be looked on before you, and the face of the youths who eat of the king's dainties; and as you see, deal with your servants." I find that word "dainties" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Then let our faces be looked on before you, and the face of the youths who eat of the king's dainties; and as you see, deal with your servants."
+Word: "dainties"
+Class: </t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>313</v>
+        <v>215</v>
       </c>
       <c r="D22" t="n">
         <v>5</v>
       </c>
       <c r="E22" t="n">
-        <v>318</v>
+        <v>220</v>
       </c>
     </row>
     <row r="23">
@@ -1007,24 +1091,28 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Wives, be in subjection to your husbands, as is fitting in the Lord." I find that word "subjection" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Wives, be in subjection to your husbands, as is fitting in the Lord."
+Word: "subjection"
+Class: </t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>294</v>
+        <v>196</v>
       </c>
       <c r="D23" t="n">
         <v>5</v>
       </c>
       <c r="E23" t="n">
-        <v>299</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24">
@@ -1033,24 +1121,28 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Yahweh has mixed a spirit of perverseness in the midst of her; and they have caused Egypt to go astray in all of its works, like a drunken man staggers in his vomit." I find that word "perverseness" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Yahweh has mixed a spirit of perverseness in the midst of her; and they have caused Egypt to go astray in all of its works, like a drunken man staggers in his vomit."
+Word: "perverseness"
+Class: </t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>320</v>
+        <v>222</v>
       </c>
       <c r="D24" t="n">
         <v>5</v>
       </c>
       <c r="E24" t="n">
-        <v>325</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25">
@@ -1059,24 +1151,28 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Multiply like grasshoppers." I find that word "grasshoppers" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Multiply like grasshoppers."
+Word: "grasshoppers"
+Class: </t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>285</v>
+        <v>187</v>
       </c>
       <c r="D25" t="n">
         <v>5</v>
       </c>
       <c r="E25" t="n">
-        <v>290</v>
+        <v>192</v>
       </c>
     </row>
     <row r="26">
@@ -1085,24 +1181,28 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Pharaoh took off his signet ring from his hand, and put it on Joseph's hand, and arrayed him in robes of fine linen, and put a gold chain about his neck," I find that word "signet" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Pharaoh took off his signet ring from his hand, and put it on Joseph's hand, and arrayed him in robes of fine linen, and put a gold chain about his neck,"
+Word: "signet"
+Class: </t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>315</v>
+        <v>217</v>
       </c>
       <c r="D26" t="n">
         <v>5</v>
       </c>
       <c r="E26" t="n">
-        <v>320</v>
+        <v>222</v>
       </c>
     </row>
     <row r="27">
@@ -1111,24 +1211,28 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "For he will deliver you from the snare of the fowler, and from the deadly pestilence." I find that word "snare" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "For he will deliver you from the snare of the fowler, and from the deadly pestilence."
+Word: "snare"
+Class: </t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>298</v>
+        <v>200</v>
       </c>
       <c r="D27" t="n">
         <v>5</v>
       </c>
       <c r="E27" t="n">
-        <v>303</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28">
@@ -1137,24 +1241,28 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "The sons of Asher: Imnah, Ishvah, Ishvi, Beriah, and Serah their sister." I find that word "Asher" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "The sons of Asher: Imnah, Ishvah, Ishvi, Beriah, and Serah their sister."
+Word: "Asher"
+Class: </t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>301</v>
+        <v>203</v>
       </c>
       <c r="D28" t="n">
         <v>5</v>
       </c>
       <c r="E28" t="n">
-        <v>306</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29">
@@ -1163,24 +1271,28 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "They sacrificed to demons, not God, to gods that they didn't know, to new gods that came up recently, which your fathers didn't dread." I find that word "demons" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "They sacrificed to demons, not God, to gods that they didn't know, to new gods that came up recently, which your fathers didn't dread."
+Word: "demons"
+Class: </t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>307</v>
+        <v>209</v>
       </c>
       <c r="D29" t="n">
         <v>5</v>
       </c>
       <c r="E29" t="n">
-        <v>312</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30">
@@ -1189,24 +1301,28 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "In the second year of Darius the king, in the sixth month, in the first day of the month, the Word of Yahweh came by Haggai, the prophet, to Zerubbabel, the son of Shealtiel, governor of Judah, and to Joshua, the son of Jehozadak, the high priest, saying," I find that word "prophet" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "In the second year of Darius the king, in the sixth month, in the first day of the month, the Word of Yahweh came by Haggai, the prophet, to Zerubbabel, the son of Shealtiel, governor of Judah, and to Joshua, the son of Jehozadak, the high priest, saying,"
+Word: "prophet"
+Class: </t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>348</v>
+        <v>250</v>
       </c>
       <c r="D30" t="n">
         <v>5</v>
       </c>
       <c r="E30" t="n">
-        <v>353</v>
+        <v>255</v>
       </c>
     </row>
     <row r="31">
@@ -1215,24 +1331,28 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "For the waters of Dimon are full of blood; for I will bring yet more on Dimon, a lion on those of Moab who escape, and on the remnant of the land." I find that word "lion" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "For the waters of Dimon are full of blood; for I will bring yet more on Dimon, a lion on those of Moab who escape, and on the remnant of the land."
+Word: "lion"
+Class: </t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>315</v>
+        <v>217</v>
       </c>
       <c r="D31" t="n">
         <v>5</v>
       </c>
       <c r="E31" t="n">
-        <v>320</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32">
@@ -1241,24 +1361,28 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>I'm reading fragments from the Bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " However, no defects in axon pathfinding along the monosynaptic reflex arc or in musclespindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).". I find that word "spindle" is neutral
-###
-I'm reading fragments from the source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment " I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.". I find that word "filthiness" is easy
-###
-I'm reading fragments from the bible, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
-After reading the fragment "Behold, the Lion who is of the tribe of Judah, the Root of David, has overcome; he who opens the book and its seven seals."" I find that word "Lion" is</t>
+          <t xml:space="preserve">I'm reading fragments from some source, and some words are not easy to understand. I'm classifying these words into "very easy", "easy", "neutral", "difficult" and "very difficult".
+Text: I will sprinkle clean water on you, and you shall be clean: from all your filthiness, and from all your idols, will I cleanse you.
+Word: filthiness
+Class: easy
+###
+Text: However, no defects in axon pathfinding along the monosynaptic reflex arc or in muscle spindle differentiation have been noted in PV KO mice, which develop normally and show no apparent changes in their behavior or physical activity (Schwaller et al. 1999).
+Word: spindle
+Class: neutral
+###
+Text: "Behold, the Lion who is of the tribe of Judah, the Root of David, has overcome; he who opens the book and its seven seals.""
+Word: "Lion"
+Class: </t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>307</v>
+        <v>209</v>
       </c>
       <c r="D32" t="n">
         <v>5</v>
       </c>
       <c r="E32" t="n">
-        <v>312</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>